<commit_message>
Update OUT data: 3 new entries added
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22900,7 +22900,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -22924,6 +22924,24 @@
       <c r="F1" t="str">
         <v>Coil No</v>
       </c>
+      <c r="G1" t="str">
+        <v>SERIAL NO</v>
+      </c>
+      <c r="H1" t="str">
+        <v>DATE &amp; TIME</v>
+      </c>
+      <c r="I1" t="str">
+        <v>VEHICLE NO</v>
+      </c>
+      <c r="J1" t="str">
+        <v>MILL COIL NO</v>
+      </c>
+      <c r="K1" t="str">
+        <v>TRANSPORTER</v>
+      </c>
+      <c r="L1" t="str">
+        <v>GROSS WT</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -22985,9 +23003,69 @@
         <v>C069328B</v>
       </c>
     </row>
+    <row r="5">
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="str">
+        <v>11-07-2025 2:09:53 PM</v>
+      </c>
+      <c r="I5" t="str">
+        <v>TN28BF2542</v>
+      </c>
+      <c r="J5" t="str">
+        <v>BCN2078C</v>
+      </c>
+      <c r="K5" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="L5">
+        <v>7455</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="str">
+        <v>11-07-2025 2:09:53 PM</v>
+      </c>
+      <c r="I6" t="str">
+        <v>TN28BF2542</v>
+      </c>
+      <c r="J6" t="str">
+        <v>C099796A</v>
+      </c>
+      <c r="K6" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="L6">
+        <v>10244</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7" t="str">
+        <v>11-07-2025 2:09:53 PM</v>
+      </c>
+      <c r="I7" t="str">
+        <v>TN28BF2542</v>
+      </c>
+      <c r="J7" t="str">
+        <v>C063616B</v>
+      </c>
+      <c r="K7" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="L7">
+        <v>10881</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 2 new entries added
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23286,67 +23286,47 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20" t="str">
-        <v>13-07-2025 7:17:51 PM</v>
+        <v>13-07-2025 7:18:38 PM</v>
       </c>
       <c r="C20" t="str">
-        <v>TN04BD9889</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D20" t="str">
-        <v>BCL6727A</v>
+        <v>C101678B</v>
       </c>
       <c r="E20" t="str">
-        <v>SJS</v>
+        <v>GWS</v>
       </c>
       <c r="F20">
-        <v>10802</v>
+        <v>10398</v>
       </c>
     </row>
     <row r="21">
       <c r="A21">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B21" t="str">
-        <v>13-07-2025 7:17:51 PM</v>
+        <v>13-07-2025 7:18:38 PM</v>
       </c>
       <c r="C21" t="str">
-        <v>TN04BD9889</v>
+        <v>TN04AR8167</v>
       </c>
       <c r="D21" t="str">
-        <v>C078765B</v>
+        <v>BCM6898A</v>
       </c>
       <c r="E21" t="str">
-        <v>SJS</v>
+        <v>GWS</v>
       </c>
       <c r="F21">
-        <v>11669</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22">
-        <v>23</v>
-      </c>
-      <c r="B22" t="str">
-        <v>13-07-2025 7:17:51 PM</v>
-      </c>
-      <c r="C22" t="str">
-        <v>TN04BD9889</v>
-      </c>
-      <c r="D22" t="str">
-        <v>BCM6898A</v>
-      </c>
-      <c r="E22" t="str">
-        <v>SJS</v>
-      </c>
-      <c r="F22">
         <v>8885</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F22"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T06:55:50.832Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23664,9 +23664,69 @@
         <v>11159</v>
       </c>
     </row>
+    <row r="39">
+      <c r="A39">
+        <v>43</v>
+      </c>
+      <c r="B39" t="str">
+        <v>15-07-2025 12:25:50 PM</v>
+      </c>
+      <c r="C39" t="str">
+        <v>TN04AS5562</v>
+      </c>
+      <c r="D39" t="str">
+        <v>C057819B</v>
+      </c>
+      <c r="E39" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F39">
+        <v>8164</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40">
+        <v>44</v>
+      </c>
+      <c r="B40" t="str">
+        <v>15-07-2025 12:25:50 PM</v>
+      </c>
+      <c r="C40" t="str">
+        <v>TN04AS5562</v>
+      </c>
+      <c r="D40" t="str">
+        <v>AS48095A</v>
+      </c>
+      <c r="E40" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F40">
+        <v>11943</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41">
+        <v>45</v>
+      </c>
+      <c r="B41" t="str">
+        <v>15-07-2025 12:25:50 PM</v>
+      </c>
+      <c r="C41" t="str">
+        <v>TN04AS5562</v>
+      </c>
+      <c r="D41" t="str">
+        <v>C101291B</v>
+      </c>
+      <c r="E41" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F41">
+        <v>9281</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F38"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T06:57:40.123Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -23669,19 +23669,19 @@
         <v>43</v>
       </c>
       <c r="B39" t="str">
-        <v>15-07-2025 12:25:50 PM</v>
+        <v>15-07-2025 12:27:40 PM</v>
       </c>
       <c r="C39" t="str">
-        <v>TN04AS5562</v>
+        <v>TN28BA6503</v>
       </c>
       <c r="D39" t="str">
-        <v>C057819B</v>
+        <v>C063616A</v>
       </c>
       <c r="E39" t="str">
-        <v>GWS</v>
+        <v>JPM</v>
       </c>
       <c r="F39">
-        <v>8164</v>
+        <v>10881</v>
       </c>
     </row>
     <row r="40">
@@ -23689,19 +23689,19 @@
         <v>44</v>
       </c>
       <c r="B40" t="str">
-        <v>15-07-2025 12:25:50 PM</v>
+        <v>15-07-2025 12:27:40 PM</v>
       </c>
       <c r="C40" t="str">
-        <v>TN04AS5562</v>
+        <v>TN28BA6503</v>
       </c>
       <c r="D40" t="str">
-        <v>AS48095A</v>
+        <v>BCL9257B</v>
       </c>
       <c r="E40" t="str">
-        <v>GWS</v>
+        <v>JPM</v>
       </c>
       <c r="F40">
-        <v>11943</v>
+        <v>10512</v>
       </c>
     </row>
     <row r="41">
@@ -23709,19 +23709,19 @@
         <v>45</v>
       </c>
       <c r="B41" t="str">
-        <v>15-07-2025 12:25:50 PM</v>
+        <v>15-07-2025 12:27:40 PM</v>
       </c>
       <c r="C41" t="str">
-        <v>TN04AS5562</v>
+        <v>TN28BA6503</v>
       </c>
       <c r="D41" t="str">
-        <v>C101291B</v>
+        <v>BCN9423A</v>
       </c>
       <c r="E41" t="str">
-        <v>GWS</v>
+        <v>JPM</v>
       </c>
       <c r="F41">
-        <v>9281</v>
+        <v>10934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T07:01:06.115Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23724,9 +23724,69 @@
         <v>10934</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42">
+        <v>46</v>
+      </c>
+      <c r="B42" t="str">
+        <v>15-07-2025 12:31:06 PM</v>
+      </c>
+      <c r="C42" t="str">
+        <v>TN03U1410</v>
+      </c>
+      <c r="D42" t="str">
+        <v>C062523B</v>
+      </c>
+      <c r="E42" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F42">
+        <v>10174</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43">
+        <v>47</v>
+      </c>
+      <c r="B43" t="str">
+        <v>15-07-2025 12:31:06 PM</v>
+      </c>
+      <c r="C43" t="str">
+        <v>TN03U1410</v>
+      </c>
+      <c r="D43" t="str">
+        <v>BCM8546C</v>
+      </c>
+      <c r="E43" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F43">
+        <v>8235</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44">
+        <v>48</v>
+      </c>
+      <c r="B44" t="str">
+        <v>15-07-2025 12:31:06 PM</v>
+      </c>
+      <c r="C44" t="str">
+        <v>TN03U1410</v>
+      </c>
+      <c r="D44" t="str">
+        <v>C078812B</v>
+      </c>
+      <c r="E44" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F44">
+        <v>11004</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F41"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F44"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T07:05:32.510Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F44"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23784,9 +23784,69 @@
         <v>11004</v>
       </c>
     </row>
+    <row r="45">
+      <c r="A45">
+        <v>49</v>
+      </c>
+      <c r="B45" t="str">
+        <v>15-07-2025 12:35:32 PM</v>
+      </c>
+      <c r="C45" t="str">
+        <v>TN03AK4559</v>
+      </c>
+      <c r="D45" t="str">
+        <v>KGK622A</v>
+      </c>
+      <c r="E45" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F45">
+        <v>11953</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46">
+        <v>50</v>
+      </c>
+      <c r="B46" t="str">
+        <v>15-07-2025 12:35:32 PM</v>
+      </c>
+      <c r="C46" t="str">
+        <v>TN03AK4559</v>
+      </c>
+      <c r="D46" t="str">
+        <v>BCM4941A</v>
+      </c>
+      <c r="E46" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F46">
+        <v>10135</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47">
+        <v>51</v>
+      </c>
+      <c r="B47" t="str">
+        <v>15-07-2025 12:35:32 PM</v>
+      </c>
+      <c r="C47" t="str">
+        <v>TN03AK4559</v>
+      </c>
+      <c r="D47" t="str">
+        <v>BCM6772A</v>
+      </c>
+      <c r="E47" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F47">
+        <v>10665</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F44"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T07:06:29.635Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -23789,19 +23789,19 @@
         <v>49</v>
       </c>
       <c r="B45" t="str">
-        <v>15-07-2025 12:35:32 PM</v>
+        <v>15-07-2025 12:36:29 PM</v>
       </c>
       <c r="C45" t="str">
-        <v>TN03AK4559</v>
+        <v>TN03U0432</v>
       </c>
       <c r="D45" t="str">
-        <v>KGK622A</v>
+        <v>BCN6657</v>
       </c>
       <c r="E45" t="str">
-        <v>MST</v>
+        <v>MPT</v>
       </c>
       <c r="F45">
-        <v>11953</v>
+        <v>13365</v>
       </c>
     </row>
     <row r="46">
@@ -23809,19 +23809,19 @@
         <v>50</v>
       </c>
       <c r="B46" t="str">
-        <v>15-07-2025 12:35:32 PM</v>
+        <v>15-07-2025 12:36:29 PM</v>
       </c>
       <c r="C46" t="str">
-        <v>TN03AK4559</v>
+        <v>TN03U0432</v>
       </c>
       <c r="D46" t="str">
-        <v>BCM4941A</v>
+        <v>BCM6772B</v>
       </c>
       <c r="E46" t="str">
-        <v>MST</v>
+        <v>MPT</v>
       </c>
       <c r="F46">
-        <v>10135</v>
+        <v>9965</v>
       </c>
     </row>
     <row r="47">
@@ -23829,19 +23829,19 @@
         <v>51</v>
       </c>
       <c r="B47" t="str">
-        <v>15-07-2025 12:35:32 PM</v>
+        <v>15-07-2025 12:36:29 PM</v>
       </c>
       <c r="C47" t="str">
-        <v>TN03AK4559</v>
+        <v>TN03U0432</v>
       </c>
       <c r="D47" t="str">
-        <v>BCM6772A</v>
+        <v>C065864A</v>
       </c>
       <c r="E47" t="str">
-        <v>MST</v>
+        <v>MPT</v>
       </c>
       <c r="F47">
-        <v>10665</v>
+        <v>8764</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 4 new entries added on 2025-07-15T07:07:38.709Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23789,19 +23789,19 @@
         <v>49</v>
       </c>
       <c r="B45" t="str">
-        <v>15-07-2025 12:36:29 PM</v>
+        <v>15-07-2025 12:37:38 PM</v>
       </c>
       <c r="C45" t="str">
-        <v>TN03U0432</v>
+        <v>TN04AH4033</v>
       </c>
       <c r="D45" t="str">
-        <v>BCN6657</v>
+        <v>BCL9256B</v>
       </c>
       <c r="E45" t="str">
-        <v>MPT</v>
+        <v>ASST</v>
       </c>
       <c r="F45">
-        <v>13365</v>
+        <v>10152</v>
       </c>
     </row>
     <row r="46">
@@ -23809,19 +23809,19 @@
         <v>50</v>
       </c>
       <c r="B46" t="str">
-        <v>15-07-2025 12:36:29 PM</v>
+        <v>15-07-2025 12:37:38 PM</v>
       </c>
       <c r="C46" t="str">
-        <v>TN03U0432</v>
+        <v>TN04AH4033</v>
       </c>
       <c r="D46" t="str">
-        <v>BCM6772B</v>
+        <v>BCM8546B</v>
       </c>
       <c r="E46" t="str">
-        <v>MPT</v>
+        <v>ASST</v>
       </c>
       <c r="F46">
-        <v>9965</v>
+        <v>8435</v>
       </c>
     </row>
     <row r="47">
@@ -23829,24 +23829,44 @@
         <v>51</v>
       </c>
       <c r="B47" t="str">
-        <v>15-07-2025 12:36:29 PM</v>
+        <v>15-07-2025 12:37:38 PM</v>
       </c>
       <c r="C47" t="str">
-        <v>TN03U0432</v>
+        <v>TN04AH4033</v>
       </c>
       <c r="D47" t="str">
-        <v>C065864A</v>
+        <v>C077440A</v>
       </c>
       <c r="E47" t="str">
-        <v>MPT</v>
+        <v>ASST</v>
       </c>
       <c r="F47">
-        <v>8764</v>
+        <v>10375</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48">
+        <v>52</v>
+      </c>
+      <c r="B48" t="str">
+        <v>15-07-2025 12:37:38 PM</v>
+      </c>
+      <c r="C48" t="str">
+        <v>TN04AH4033</v>
+      </c>
+      <c r="D48" t="str">
+        <v>C087504A</v>
+      </c>
+      <c r="E48" t="str">
+        <v>ASST</v>
+      </c>
+      <c r="F48">
+        <v>9915</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F47"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F48"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T07:09:35.782Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23789,19 +23789,19 @@
         <v>49</v>
       </c>
       <c r="B45" t="str">
-        <v>15-07-2025 12:37:38 PM</v>
+        <v>15-07-2025 12:39:35 PM</v>
       </c>
       <c r="C45" t="str">
-        <v>TN04AH4033</v>
+        <v>TN04AM7632</v>
       </c>
       <c r="D45" t="str">
-        <v>BCL9256B</v>
+        <v>BCM8546C</v>
       </c>
       <c r="E45" t="str">
-        <v>ASST</v>
+        <v>GWS</v>
       </c>
       <c r="F45">
-        <v>10152</v>
+        <v>8235</v>
       </c>
     </row>
     <row r="46">
@@ -23809,19 +23809,19 @@
         <v>50</v>
       </c>
       <c r="B46" t="str">
-        <v>15-07-2025 12:37:38 PM</v>
+        <v>15-07-2025 12:39:35 PM</v>
       </c>
       <c r="C46" t="str">
-        <v>TN04AH4033</v>
+        <v>TN04AM7632</v>
       </c>
       <c r="D46" t="str">
-        <v>BCM8546B</v>
+        <v>KGK695A</v>
       </c>
       <c r="E46" t="str">
-        <v>ASST</v>
+        <v>GWS</v>
       </c>
       <c r="F46">
-        <v>8435</v>
+        <v>12443</v>
       </c>
     </row>
     <row r="47">
@@ -23829,44 +23829,24 @@
         <v>51</v>
       </c>
       <c r="B47" t="str">
-        <v>15-07-2025 12:37:38 PM</v>
+        <v>15-07-2025 12:39:35 PM</v>
       </c>
       <c r="C47" t="str">
-        <v>TN04AH4033</v>
+        <v>TN04AM7632</v>
       </c>
       <c r="D47" t="str">
-        <v>C077440A</v>
+        <v>C071955</v>
       </c>
       <c r="E47" t="str">
-        <v>ASST</v>
+        <v>GWS</v>
       </c>
       <c r="F47">
-        <v>10375</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48">
-        <v>52</v>
-      </c>
-      <c r="B48" t="str">
-        <v>15-07-2025 12:37:38 PM</v>
-      </c>
-      <c r="C48" t="str">
-        <v>TN04AH4033</v>
-      </c>
-      <c r="D48" t="str">
-        <v>C087504A</v>
-      </c>
-      <c r="E48" t="str">
-        <v>ASST</v>
-      </c>
-      <c r="F48">
-        <v>9915</v>
+        <v>10894</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F48"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F47"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T07:22:33.139Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23844,9 +23844,69 @@
         <v>10894</v>
       </c>
     </row>
+    <row r="48">
+      <c r="A48">
+        <v>52</v>
+      </c>
+      <c r="B48" t="str">
+        <v>15-07-2025 12:52:32 PM</v>
+      </c>
+      <c r="C48" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D48" t="str">
+        <v>BCN2078A</v>
+      </c>
+      <c r="E48" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F48">
+        <v>7635</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49">
+        <v>53</v>
+      </c>
+      <c r="B49" t="str">
+        <v>15-07-2025 12:52:32 PM</v>
+      </c>
+      <c r="C49" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D49" t="str">
+        <v>C087506B</v>
+      </c>
+      <c r="E49" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F49">
+        <v>11159</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50">
+        <v>54</v>
+      </c>
+      <c r="B50" t="str">
+        <v>15-07-2025 12:52:32 PM</v>
+      </c>
+      <c r="C50" t="str">
+        <v>TN04AR8167</v>
+      </c>
+      <c r="D50" t="str">
+        <v>C065864A</v>
+      </c>
+      <c r="E50" t="str">
+        <v>GWS</v>
+      </c>
+      <c r="F50">
+        <v>8764</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F47"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F50"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-15T07:45:36.859Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -23904,9 +23904,69 @@
         <v>8764</v>
       </c>
     </row>
+    <row r="51">
+      <c r="A51">
+        <v>55</v>
+      </c>
+      <c r="B51" t="str">
+        <v>15-07-2025 1:15:36 PM</v>
+      </c>
+      <c r="C51" t="str">
+        <v>TN03AK4559</v>
+      </c>
+      <c r="D51" t="str">
+        <v>BCN6657</v>
+      </c>
+      <c r="E51" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F51">
+        <v>13365</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52">
+        <v>56</v>
+      </c>
+      <c r="B52" t="str">
+        <v>15-07-2025 1:15:36 PM</v>
+      </c>
+      <c r="C52" t="str">
+        <v>TN03AK4559</v>
+      </c>
+      <c r="D52" t="str">
+        <v>BCM6891C</v>
+      </c>
+      <c r="E52" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F52">
+        <v>8705</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53">
+        <v>57</v>
+      </c>
+      <c r="B53" t="str">
+        <v>15-07-2025 1:15:36 PM</v>
+      </c>
+      <c r="C53" t="str">
+        <v>TN03AK4559</v>
+      </c>
+      <c r="D53" t="str">
+        <v>BCM3462B</v>
+      </c>
+      <c r="E53" t="str">
+        <v>MST</v>
+      </c>
+      <c r="F53">
+        <v>8875</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F50"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F53"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T06:31:18.694Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F56"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24024,9 +24024,69 @@
         <v>11841</v>
       </c>
     </row>
+    <row r="57">
+      <c r="A57">
+        <v>64</v>
+      </c>
+      <c r="B57" t="str">
+        <v>16-07-2025 12:01:18 PM</v>
+      </c>
+      <c r="C57" t="str">
+        <v>TN04P4876</v>
+      </c>
+      <c r="D57" t="str">
+        <v>BCM6888C</v>
+      </c>
+      <c r="E57" t="str">
+        <v>MSMD</v>
+      </c>
+      <c r="F57">
+        <v>8355</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58">
+        <v>65</v>
+      </c>
+      <c r="B58" t="str">
+        <v>16-07-2025 12:01:18 PM</v>
+      </c>
+      <c r="C58" t="str">
+        <v>TN04P4876</v>
+      </c>
+      <c r="D58" t="str">
+        <v>C073932B</v>
+      </c>
+      <c r="E58" t="str">
+        <v>MSMD</v>
+      </c>
+      <c r="F58">
+        <v>8034</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59">
+        <v>66</v>
+      </c>
+      <c r="B59" t="str">
+        <v>16-07-2025 12:01:18 PM</v>
+      </c>
+      <c r="C59" t="str">
+        <v>TN04P4876</v>
+      </c>
+      <c r="D59" t="str">
+        <v>BCN2078C</v>
+      </c>
+      <c r="E59" t="str">
+        <v>MSMD</v>
+      </c>
+      <c r="F59">
+        <v>7455</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F56"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F59"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T06:46:28.362Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24084,9 +24084,69 @@
         <v>7455</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60">
+        <v>67</v>
+      </c>
+      <c r="B60" t="str">
+        <v>16-07-2025 12:16:28 PM</v>
+      </c>
+      <c r="C60" t="str">
+        <v>TN28AL5969</v>
+      </c>
+      <c r="D60" t="str">
+        <v>C100526A</v>
+      </c>
+      <c r="E60" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F60">
+        <v>10148</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61">
+        <v>68</v>
+      </c>
+      <c r="B61" t="str">
+        <v>16-07-2025 12:16:28 PM</v>
+      </c>
+      <c r="C61" t="str">
+        <v>TN28AL5969</v>
+      </c>
+      <c r="D61" t="str">
+        <v>BCM7923B</v>
+      </c>
+      <c r="E61" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F61">
+        <v>8915</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62">
+        <v>69</v>
+      </c>
+      <c r="B62" t="str">
+        <v>16-07-2025 12:16:28 PM</v>
+      </c>
+      <c r="C62" t="str">
+        <v>TN28AL5969</v>
+      </c>
+      <c r="D62" t="str">
+        <v>C065863C</v>
+      </c>
+      <c r="E62" t="str">
+        <v>SKT</v>
+      </c>
+      <c r="F62">
+        <v>8644</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F59"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F62"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update OUT data: 3 new entries added on 2025-07-16T06:48:28.901Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -24089,19 +24089,19 @@
         <v>67</v>
       </c>
       <c r="B60" t="str">
-        <v>16-07-2025 12:16:28 PM</v>
+        <v>16-07-2025 12:18:28 PM</v>
       </c>
       <c r="C60" t="str">
-        <v>TN28AL5969</v>
+        <v>TN04AH3326</v>
       </c>
       <c r="D60" t="str">
-        <v>C100526A</v>
+        <v>C075553A</v>
       </c>
       <c r="E60" t="str">
-        <v>SKT</v>
+        <v>SAI</v>
       </c>
       <c r="F60">
-        <v>10148</v>
+        <v>10758</v>
       </c>
     </row>
     <row r="61">
@@ -24109,19 +24109,19 @@
         <v>68</v>
       </c>
       <c r="B61" t="str">
-        <v>16-07-2025 12:16:28 PM</v>
+        <v>16-07-2025 12:18:28 PM</v>
       </c>
       <c r="C61" t="str">
-        <v>TN28AL5969</v>
+        <v>TN04AH3326</v>
       </c>
       <c r="D61" t="str">
-        <v>BCM7923B</v>
+        <v>BCM4917A</v>
       </c>
       <c r="E61" t="str">
-        <v>SKT</v>
+        <v>SAI</v>
       </c>
       <c r="F61">
-        <v>8915</v>
+        <v>7265</v>
       </c>
     </row>
     <row r="62">
@@ -24129,19 +24129,19 @@
         <v>69</v>
       </c>
       <c r="B62" t="str">
-        <v>16-07-2025 12:16:28 PM</v>
+        <v>16-07-2025 12:18:28 PM</v>
       </c>
       <c r="C62" t="str">
-        <v>TN28AL5969</v>
+        <v>TN04AH3326</v>
       </c>
       <c r="D62" t="str">
-        <v>C065863C</v>
+        <v>C077440A</v>
       </c>
       <c r="E62" t="str">
-        <v>SKT</v>
+        <v>SAI</v>
       </c>
       <c r="F62">
-        <v>8644</v>
+        <v>10375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update OUT data: 4 new entries added on 2025-07-16T06:58:04.618Z
</commit_message>
<xml_diff>
--- a/coil-data.xlsx
+++ b/coil-data.xlsx
@@ -22899,7 +22899,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F62"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -24144,9 +24144,89 @@
         <v>10375</v>
       </c>
     </row>
+    <row r="63">
+      <c r="A63">
+        <v>73</v>
+      </c>
+      <c r="B63" t="str">
+        <v>16-07-2025 12:28:04 PM</v>
+      </c>
+      <c r="C63" t="str">
+        <v>TN03U0432</v>
+      </c>
+      <c r="D63" t="str">
+        <v>C101527A</v>
+      </c>
+      <c r="E63" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F63">
+        <v>12209</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64">
+        <v>74</v>
+      </c>
+      <c r="B64" t="str">
+        <v>16-07-2025 12:28:04 PM</v>
+      </c>
+      <c r="C64" t="str">
+        <v>TN03U0432</v>
+      </c>
+      <c r="D64" t="str">
+        <v>C063616B</v>
+      </c>
+      <c r="E64" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F64">
+        <v>10881</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65">
+        <v>75</v>
+      </c>
+      <c r="B65" t="str">
+        <v>16-07-2025 12:28:04 PM</v>
+      </c>
+      <c r="C65" t="str">
+        <v>TN03U0432</v>
+      </c>
+      <c r="D65" t="str">
+        <v>C100211A</v>
+      </c>
+      <c r="E65" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F65">
+        <v>7015</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66">
+        <v>76</v>
+      </c>
+      <c r="B66" t="str">
+        <v>16-07-2025 12:28:04 PM</v>
+      </c>
+      <c r="C66" t="str">
+        <v>TN03U0432</v>
+      </c>
+      <c r="D66" t="str">
+        <v>C065863C</v>
+      </c>
+      <c r="E66" t="str">
+        <v>MPT</v>
+      </c>
+      <c r="F66">
+        <v>8644</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F62"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F66"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>